<commit_message>
update: added generate report route
</commit_message>
<xml_diff>
--- a/user-device-data/generatedReport.xlsx
+++ b/user-device-data/generatedReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Devices Last data Points Report</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Report Generated At</t>
   </si>
   <si>
-    <t>12/27/2023, 4:03:24 PM</t>
+    <t>12/27/2023, 9:58:55 PM</t>
   </si>
   <si>
     <t>Device Name</t>
@@ -46,12 +46,18 @@
     <t>ACTIVE</t>
   </si>
   <si>
+    <t>74.95 KW</t>
+  </si>
+  <si>
     <t>12/26/2023, 8:31:18 PM</t>
   </si>
   <si>
     <t>CUR1</t>
   </si>
   <si>
+    <t>24.05 A</t>
+  </si>
+  <si>
     <t>CUR2</t>
   </si>
   <si>
@@ -61,15 +67,27 @@
     <t>FREQ</t>
   </si>
   <si>
+    <t>24.05 Hz</t>
+  </si>
+  <si>
     <t>MD</t>
   </si>
   <si>
+    <t>24.05 KVAr</t>
+  </si>
+  <si>
     <t>MDKW</t>
   </si>
   <si>
+    <t>24.05 KW</t>
+  </si>
+  <si>
     <t>PF1</t>
   </si>
   <si>
+    <t xml:space="preserve">1.00 </t>
+  </si>
+  <si>
     <t>PF2</t>
   </si>
   <si>
@@ -85,7 +103,13 @@
     <t>RSSI</t>
   </si>
   <si>
+    <t xml:space="preserve">22.00 </t>
+  </si>
+  <si>
     <t>VOLTS1</t>
+  </si>
+  <si>
+    <t>24.05 V</t>
   </si>
   <si>
     <t>VOLTS2</t>
@@ -127,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -135,11 +159,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -148,6 +185,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,286 +558,253 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
-        <v>74.9518915362767</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="1">
-        <v>24.04515701926204</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
+      <c r="D22" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A23" s="5"/>
       <c r="B23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="1">
-        <v>24.04515701926204</v>
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
   <headerFooter>

</xml_diff>